<commit_message>
feat: add price db, dynamic data for fan database
</commit_message>
<xml_diff>
--- a/pdf-test/test.xlsx
+++ b/pdf-test/test.xlsx
@@ -1,24 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24332"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86C8AF71-63F3-4F20-9364-72F41671CFC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet sheetId="1" name="Техника" state="visible" r:id="rId4"/>
+    <sheet name="Техника" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Техника'!$A1:$K156</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="0">'Техника'!$1:$6</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">Техника!$1:$6</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Техника!$A$1:$K$156</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="58">
   <si>
     <t>Версия программы: 1.0.0</t>
   </si>
@@ -183,57 +184,66 @@
   </si>
   <si>
     <t>Схемы</t>
+  </si>
+  <si>
+    <t>asdasd</t>
+  </si>
+  <si>
+    <t>adsdadsa</t>
+  </si>
+  <si>
+    <t>daasdas</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-      <sz val="11"/>
-      <name val="Calibri"/>
     </font>
     <font>
+      <sz val="12"/>
       <color theme="0" tint="-0.34931485946226387"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-      <sz val="12"/>
-      <name val="Calibri"/>
     </font>
     <font>
       <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <charset val="204"/>
-      <color theme="1"/>
-      <family val="2"/>
       <scheme val="minor"/>
-      <sz val="16"/>
-      <name val="Calibri"/>
     </font>
     <font>
+      <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
       <family val="2"/>
-      <sz val="11"/>
-      <name val="Calibri"/>
     </font>
     <font>
       <b/>
+      <sz val="12"/>
       <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
       <family val="2"/>
-      <sz val="12"/>
-      <name val="Calibri"/>
     </font>
     <font>
       <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <charset val="204"/>
-      <color theme="0"/>
-      <family val="2"/>
       <scheme val="minor"/>
-      <sz val="12"/>
-      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="6">
@@ -251,7 +261,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.7999206518753624"/>
+        <fgColor theme="4" tint="0.79992065187536243"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -263,7 +273,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.7999511703848384"/>
+        <fgColor theme="4" tint="0.79995117038483843"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -280,49 +290,28 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -338,16 +327,7 @@
     <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -375,9 +355,48 @@
     <xf numFmtId="1" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -409,7 +428,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="1" name="Picture 1">
+        <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
@@ -453,10 +472,10 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 2">
+        <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -497,10 +516,10 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 3">
+        <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -541,10 +560,10 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 4">
+        <xdr:cNvPr id="5" name="Picture 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -585,10 +604,10 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Picture 5">
+        <xdr:cNvPr id="6" name="Picture 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -629,10 +648,10 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Picture 6">
+        <xdr:cNvPr id="7" name="Picture 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -673,10 +692,10 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="7" name="Picture 7">
+        <xdr:cNvPr id="8" name="Picture 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -717,10 +736,10 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="8" name="Picture 8">
+        <xdr:cNvPr id="9" name="Picture 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -761,10 +780,10 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="9" name="Picture 9">
+        <xdr:cNvPr id="10" name="Picture 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -805,10 +824,10 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="10" name="Picture 10">
+        <xdr:cNvPr id="11" name="Picture 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -849,10 +868,10 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="11" name="Picture 11">
+        <xdr:cNvPr id="12" name="Picture 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -893,10 +912,10 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="12" name="Picture 12">
+        <xdr:cNvPr id="13" name="Picture 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -937,10 +956,10 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="13" name="Picture 13">
+        <xdr:cNvPr id="14" name="Picture 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1231,656 +1250,668 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K107"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100" view="pageBreakPreview">
-      <selection activeCell="E136" sqref="E136"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A39" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A53" sqref="A53:XFD53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.3" customHeight="1"/>
+  <sheetFormatPr defaultRowHeight="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="11" max="11" width="10.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="16.05" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-    </row>
-    <row r="2" ht="16.05" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="1" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="24"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+    </row>
+    <row r="2" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-    </row>
-    <row r="3" ht="16.05" customHeight="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="5"/>
-    </row>
-    <row r="4" ht="16.05" customHeight="1" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C4" s="6"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="H4" s="8" t="s">
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+    </row>
+    <row r="3" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="1"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="26"/>
+      <c r="K3" s="26"/>
+    </row>
+    <row r="4" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C4" s="3"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="H4" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="I4" s="8"/>
-      <c r="J4" s="9"/>
-      <c r="K4" s="9"/>
-    </row>
-    <row r="5" ht="16.05" customHeight="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="10"/>
-      <c r="B5" s="10"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="7" t="s">
+      <c r="I4" s="28"/>
+      <c r="J4" s="29"/>
+      <c r="K4" s="29"/>
+    </row>
+    <row r="5" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="I5" s="7"/>
-      <c r="J5" s="12">
-        <v>45320.16092658565</v>
-      </c>
-      <c r="K5" s="12"/>
-    </row>
-    <row r="6" ht="16.05" customHeight="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="13"/>
-      <c r="B6" s="13"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="13"/>
-      <c r="I6" s="13"/>
-      <c r="J6" s="13"/>
-      <c r="K6" s="13"/>
-    </row>
-    <row r="7" ht="16.05" customHeight="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="15" t="s">
+      <c r="I5" s="4"/>
+      <c r="J5" s="30">
+        <v>45320.160926585653</v>
+      </c>
+      <c r="K5" s="30"/>
+    </row>
+    <row r="6" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="7"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
+    </row>
+    <row r="7" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="15"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="15"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="15"/>
-      <c r="H7" s="15"/>
-      <c r="I7" s="15"/>
-      <c r="J7" s="15"/>
-      <c r="K7" s="15"/>
-    </row>
-    <row r="8" ht="16.05" customHeight="1" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B8" s="16"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="16"/>
-      <c r="H8" s="16"/>
-      <c r="I8" s="16"/>
-      <c r="J8" s="16"/>
-      <c r="K8" s="16"/>
-    </row>
-    <row r="9" ht="16.05" customHeight="1" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B9" s="8" t="s">
+      <c r="B7" s="31"/>
+      <c r="C7" s="31"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="31"/>
+      <c r="F7" s="31"/>
+      <c r="G7" s="31"/>
+      <c r="H7" s="31"/>
+      <c r="I7" s="31"/>
+      <c r="J7" s="31"/>
+      <c r="K7" s="31"/>
+    </row>
+    <row r="8" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+    </row>
+    <row r="9" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="17" t="s">
+      <c r="C9" s="28"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="F9" s="17"/>
-      <c r="G9" s="18"/>
-      <c r="H9" s="18" t="s">
+      <c r="F9" s="32"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="I9" s="17"/>
-      <c r="J9" s="17">
+      <c r="I9" s="10"/>
+      <c r="J9" s="10">
         <v>618</v>
       </c>
-      <c r="K9" s="19"/>
-    </row>
-    <row r="10" ht="16.05" customHeight="1" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B10" s="8" t="s">
+      <c r="K9" s="12"/>
+    </row>
+    <row r="10" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="17" t="s">
+      <c r="C10" s="28"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="F10" s="17"/>
-      <c r="G10" s="18"/>
-      <c r="H10" s="18" t="s">
+      <c r="F10" s="32"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="I10" s="17"/>
-      <c r="J10" s="17">
+      <c r="I10" s="10"/>
+      <c r="J10" s="10">
         <v>435</v>
       </c>
-      <c r="K10" s="19"/>
-    </row>
-    <row r="11" ht="16.05" customHeight="1" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B11" s="8" t="s">
+      <c r="K10" s="12"/>
+    </row>
+    <row r="11" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="17" t="s">
+      <c r="C11" s="28"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="F11" s="17"/>
-      <c r="G11" s="18"/>
-      <c r="H11" s="18" t="s">
+      <c r="F11" s="32"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="I11" s="17"/>
-      <c r="J11" s="17">
+      <c r="I11" s="10"/>
+      <c r="J11" s="10">
         <v>618</v>
       </c>
-      <c r="K11" s="19"/>
-    </row>
-    <row r="12" ht="16.05" customHeight="1" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B12" s="8" t="s">
+      <c r="K11" s="12"/>
+    </row>
+    <row r="12" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="17" t="s">
+      <c r="C12" s="28"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="F12" s="17"/>
-      <c r="G12" s="18"/>
-      <c r="H12" s="18" t="s">
+      <c r="F12" s="32"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="I12" s="17"/>
-      <c r="J12" s="20">
+      <c r="I12" s="10"/>
+      <c r="J12" s="13">
         <f>G24+H68+H80+H92+H104+H116+H128</f>
-        <v>0</v>
-      </c>
-      <c r="K12" s="19"/>
-    </row>
-    <row r="13" ht="16.05" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="14" ht="16.05" customHeight="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="K12" s="12"/>
+    </row>
+    <row r="13" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="21"/>
-      <c r="C14" s="21"/>
-      <c r="D14" s="21"/>
-      <c r="E14" s="21"/>
-      <c r="F14" s="21"/>
-      <c r="G14" s="21"/>
-      <c r="H14" s="21"/>
-      <c r="I14" s="21"/>
-      <c r="J14" s="21"/>
-      <c r="K14" s="21"/>
-    </row>
-    <row r="15" ht="16.05" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="16" ht="16.05" customHeight="1" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B16" s="22" t="s">
+      <c r="B14" s="33"/>
+      <c r="C14" s="33"/>
+      <c r="D14" s="33"/>
+      <c r="E14" s="33"/>
+      <c r="F14" s="33"/>
+      <c r="G14" s="33"/>
+      <c r="H14" s="33"/>
+      <c r="I14" s="33"/>
+      <c r="J14" s="33"/>
+      <c r="K14" s="33"/>
+    </row>
+    <row r="15" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="22"/>
-      <c r="D16" s="22"/>
-      <c r="E16" s="23" t="s">
+      <c r="C16" s="34"/>
+      <c r="D16" s="34"/>
+      <c r="E16" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="F16" s="23"/>
-      <c r="G16" s="23"/>
-    </row>
-    <row r="17" ht="16.05" customHeight="1" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B17" s="22" t="s">
+      <c r="F16" s="35"/>
+      <c r="G16" s="35"/>
+    </row>
+    <row r="17" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="C17" s="22"/>
-      <c r="D17" s="22"/>
-      <c r="E17" s="23"/>
-      <c r="F17" s="23" t="s">
+      <c r="C17" s="34"/>
+      <c r="D17" s="34"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="G17" s="23"/>
-    </row>
-    <row r="18" ht="16.05" customHeight="1" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="22" t="s">
+      <c r="G17" s="35"/>
+    </row>
+    <row r="18" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="C18" s="22"/>
-      <c r="D18" s="22"/>
-      <c r="E18" s="24" t="s">
+      <c r="C18" s="34"/>
+      <c r="D18" s="34"/>
+      <c r="E18" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="F18" s="24"/>
-      <c r="G18" s="24"/>
-    </row>
-    <row r="19" ht="16.05" customHeight="1" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B19" s="7" t="s">
+      <c r="F18" s="36"/>
+      <c r="G18" s="36"/>
+    </row>
+    <row r="19" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E19" s="25"/>
-      <c r="F19" s="25"/>
-      <c r="G19" s="25" t="s">
+      <c r="E19" s="15"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="15" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="20" ht="16.05" customHeight="1" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B20" s="7" t="s">
+    <row r="20" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="E20" s="25"/>
-      <c r="F20" s="25"/>
-      <c r="G20" s="25">
+      <c r="E20" s="15"/>
+      <c r="F20" s="15"/>
+      <c r="G20" s="15">
         <v>0.38</v>
       </c>
     </row>
-    <row r="21" ht="16.05" customHeight="1" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B21" s="7" t="s">
+    <row r="21" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E21" s="25"/>
-      <c r="F21" s="25"/>
-      <c r="G21" s="25">
+      <c r="E21" s="15"/>
+      <c r="F21" s="15"/>
+      <c r="G21" s="15">
         <v>1.7</v>
       </c>
     </row>
-    <row r="22" ht="16.05" customHeight="1" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B22" s="7" t="s">
+    <row r="22" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="E22" s="25"/>
-      <c r="F22" s="25"/>
-      <c r="G22" s="25">
+      <c r="E22" s="15"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="15">
         <v>1420</v>
       </c>
     </row>
-    <row r="23" ht="16.05" customHeight="1" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B23" s="7" t="s">
+    <row r="23" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="E23" s="25"/>
-      <c r="F23" s="25"/>
-      <c r="G23" s="25" t="s">
+      <c r="E23" s="15"/>
+      <c r="F23" s="15"/>
+      <c r="G23" s="15" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="24" ht="16.05" customHeight="1" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B24" s="7" t="s">
+    <row r="24" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="E24" s="25"/>
-      <c r="F24" s="25"/>
-      <c r="G24" s="26">
+      <c r="E24" s="15"/>
+      <c r="F24" s="15"/>
+      <c r="G24" s="16">
         <v>32</v>
       </c>
     </row>
-    <row r="25" ht="16.05" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B25" s="27"/>
-    </row>
-    <row r="26" ht="16.05" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="27" ht="16.05" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" ht="16.05" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="29" ht="16.05" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" ht="16.05" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" ht="16.05" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" ht="16.05" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="33" ht="16.05" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="34" ht="16.05" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="35" ht="16.05" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="36" ht="16.05" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="37" ht="16.05" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="38" ht="16.05" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="39" ht="16.05" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="40" ht="16.05" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="41" ht="16.05" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="42" ht="16.05" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="43" ht="16.05" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="17"/>
+    </row>
+    <row r="26" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="27" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="28" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="29" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="30" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="31" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="32" spans="2:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="33" spans="2:10" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="34" spans="2:10" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="35" spans="2:10" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="36" spans="2:10" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="37" spans="2:10" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="38" spans="2:10" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="39" spans="2:10" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="40" spans="2:10" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="41" spans="2:10" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="42" spans="2:10" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="43" spans="2:10" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B43" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="44" ht="16.05" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="45" ht="16.05" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="46" ht="16.05" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="47" ht="16.05" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="48" ht="16.05" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="49" ht="16.05" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="50" ht="16.05" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="51" ht="16.05" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="52" ht="16.05" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="53" ht="16.05" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="54" ht="16.05" customHeight="1" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B54" s="28" t="s">
+    <row r="44" spans="2:10" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I44" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="45" spans="2:10" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="46" spans="2:10" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H46" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="47" spans="2:10" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J47" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="48" spans="2:10" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="49" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="50" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="51" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="52" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="53" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="54" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B54" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="C54" s="28" t="s">
+      <c r="C54" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="D54" s="28" t="s">
+      <c r="D54" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="E54" s="28" t="s">
+      <c r="E54" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="F54" s="28" t="s">
+      <c r="F54" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="G54" s="28" t="s">
+      <c r="G54" s="18" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="55" ht="16.05" customHeight="1" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B55" s="29">
+    <row r="55" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B55" s="19">
         <v>720</v>
       </c>
-      <c r="C55" s="29">
+      <c r="C55" s="19">
         <v>618</v>
       </c>
-      <c r="D55" s="29">
+      <c r="D55" s="19">
         <v>595</v>
       </c>
-      <c r="E55" s="29">
+      <c r="E55" s="19">
         <v>435</v>
       </c>
-      <c r="F55" s="30" t="s">
+      <c r="F55" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="G55" s="29">
+      <c r="G55" s="19">
         <v>450</v>
       </c>
     </row>
-    <row r="56" ht="16.05" customHeight="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A56" s="21" t="s">
+    <row r="56" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="B56" s="21"/>
-      <c r="C56" s="21"/>
-      <c r="D56" s="21"/>
-      <c r="E56" s="21"/>
-      <c r="F56" s="21"/>
-      <c r="G56" s="21"/>
-      <c r="H56" s="21"/>
-      <c r="I56" s="21"/>
-      <c r="J56" s="21"/>
-      <c r="K56" s="21"/>
-    </row>
-    <row r="57" ht="16.05" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="58" ht="16.05" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B56" s="33"/>
+      <c r="C56" s="33"/>
+      <c r="D56" s="33"/>
+      <c r="E56" s="33"/>
+      <c r="F56" s="33"/>
+      <c r="G56" s="33"/>
+      <c r="H56" s="33"/>
+      <c r="I56" s="33"/>
+      <c r="J56" s="33"/>
+      <c r="K56" s="33"/>
+    </row>
+    <row r="57" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="58" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B58" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="59" ht="16.05" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="60" ht="16.05" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="61" ht="16.05" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="62" ht="16.05" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="63" ht="16.05" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="64" ht="16.05" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="65" ht="16.05" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="66" ht="16.05" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="67" ht="16.05" customHeight="1" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B67" s="28" t="s">
+    <row r="59" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="60" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="61" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="62" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="63" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="64" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="65" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="66" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="67" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B67" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="C67" s="28" t="s">
+      <c r="C67" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="D67" s="28" t="s">
+      <c r="D67" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="E67" s="28" t="s">
+      <c r="E67" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="F67" s="28" t="s">
+      <c r="F67" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="G67" s="28" t="s">
+      <c r="G67" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="H67" s="28" t="s">
+      <c r="H67" s="18" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="68" ht="16.05" customHeight="1" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B68" s="31">
+    <row r="68" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B68" s="21">
         <v>450</v>
       </c>
-      <c r="C68" s="31">
+      <c r="C68" s="21">
         <v>575</v>
       </c>
-      <c r="D68" s="28" t="s">
+      <c r="D68" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="E68" s="31">
+      <c r="E68" s="21">
         <v>475</v>
       </c>
-      <c r="F68" s="31">
+      <c r="F68" s="21">
         <v>817</v>
       </c>
-      <c r="G68" s="31">
+      <c r="G68" s="21">
         <v>300</v>
       </c>
-      <c r="H68" s="31">
+      <c r="H68" s="21">
         <v>10</v>
       </c>
     </row>
-    <row r="69" ht="16.05" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="70" ht="16.05" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="70" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B70" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="71" ht="16.05" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="72" ht="16.05" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="73" ht="16.05" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="74" ht="16.05" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="75" ht="16.05" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="76" ht="16.05" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="77" ht="16.05" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="78" ht="16.05" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="79" ht="16.05" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B79" s="32" t="s">
+    <row r="71" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="72" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="73" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="74" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="75" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="76" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="77" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="78" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="79" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B79" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="C79" s="32" t="s">
+      <c r="C79" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="D79" s="32" t="s">
+      <c r="D79" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="E79" s="32" t="s">
+      <c r="E79" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="F79" s="32"/>
-      <c r="G79" s="32"/>
-      <c r="H79" s="32" t="s">
+      <c r="F79" s="22"/>
+      <c r="G79" s="22"/>
+      <c r="H79" s="22" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="80" ht="16.05" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B80" s="33">
+    <row r="80" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B80" s="23">
         <v>438</v>
       </c>
-      <c r="C80" s="33">
+      <c r="C80" s="23">
         <v>402</v>
       </c>
-      <c r="D80" s="33">
+      <c r="D80" s="23">
         <v>464</v>
       </c>
-      <c r="E80" s="33">
+      <c r="E80" s="23">
         <v>220</v>
       </c>
-      <c r="F80" s="33"/>
-      <c r="G80" s="33"/>
-      <c r="H80" s="33">
+      <c r="F80" s="23"/>
+      <c r="G80" s="23"/>
+      <c r="H80" s="23">
         <v>1</v>
       </c>
     </row>
-    <row r="81" ht="16.05" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="82" ht="16.05" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="82" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B82" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="83" ht="16.05" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="84" ht="16.05" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="85" ht="16.05" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="86" ht="16.05" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="87" ht="16.05" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="88" ht="16.05" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="89" ht="16.05" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="90" ht="16.05" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="91" ht="16.05" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B91" s="28" t="s">
+    <row r="83" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="84" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="85" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="86" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="87" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="88" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="89" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="90" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="91" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B91" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="C91" s="28" t="s">
+      <c r="C91" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="D91" s="28" t="s">
+      <c r="D91" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="E91" s="28"/>
-      <c r="F91" s="28"/>
-      <c r="G91" s="28"/>
-      <c r="H91" s="28" t="s">
+      <c r="E91" s="18"/>
+      <c r="F91" s="18"/>
+      <c r="G91" s="18"/>
+      <c r="H91" s="18" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="92" ht="16.05" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B92" s="31">
+    <row r="92" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B92" s="21">
         <v>400</v>
       </c>
-      <c r="C92" s="31">
+      <c r="C92" s="21">
         <v>438</v>
       </c>
-      <c r="D92" s="31">
+      <c r="D92" s="21">
         <v>464</v>
       </c>
-      <c r="E92" s="31"/>
-      <c r="F92" s="31"/>
-      <c r="G92" s="31"/>
-      <c r="H92" s="31">
+      <c r="E92" s="21"/>
+      <c r="F92" s="21"/>
+      <c r="G92" s="21"/>
+      <c r="H92" s="21">
         <v>2</v>
       </c>
     </row>
-    <row r="93" ht="16.05" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="94" ht="16.05" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="94" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B94" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="95" ht="16.05" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="96" ht="16.05" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="97" ht="16.05" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="98" ht="16.05" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="99" ht="16.05" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="100" ht="16.05" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="101" ht="16.05" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="102" ht="16.05" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="103" ht="16.05" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B103" s="32" t="s">
+    <row r="95" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="96" spans="2:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="97" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="98" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="99" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="100" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="101" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="102" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="103" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B103" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="C103" s="32" t="s">
+      <c r="C103" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="D103" s="32" t="s">
+      <c r="D103" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="E103" s="32" t="s">
+      <c r="E103" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="F103" s="32"/>
-      <c r="G103" s="32"/>
-      <c r="H103" s="32" t="s">
+      <c r="F103" s="22"/>
+      <c r="G103" s="22"/>
+      <c r="H103" s="22" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="104" ht="16.05" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B104" s="33">
+    <row r="104" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B104" s="23">
         <v>400</v>
       </c>
-      <c r="C104" s="33">
+      <c r="C104" s="23">
         <v>438</v>
       </c>
-      <c r="D104" s="33">
+      <c r="D104" s="23">
         <v>464</v>
       </c>
-      <c r="E104" s="33">
+      <c r="E104" s="23">
         <v>75</v>
       </c>
-      <c r="F104" s="33"/>
-      <c r="G104" s="33"/>
-      <c r="H104" s="33">
+      <c r="F104" s="23"/>
+      <c r="G104" s="23"/>
+      <c r="H104" s="23">
         <v>2</v>
       </c>
     </row>
-    <row r="106" ht="16.05" customHeight="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A106" s="21" t="s">
+    <row r="106" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A106" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="B106" s="21"/>
-      <c r="C106" s="21"/>
-      <c r="D106" s="21"/>
-      <c r="E106" s="21"/>
-      <c r="F106" s="21"/>
-      <c r="G106" s="21"/>
-      <c r="H106" s="21"/>
-      <c r="I106" s="21"/>
-      <c r="J106" s="21"/>
-      <c r="K106" s="21"/>
-    </row>
-    <row r="107" ht="16.05" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="B106" s="33"/>
+      <c r="C106" s="33"/>
+      <c r="D106" s="33"/>
+      <c r="E106" s="33"/>
+      <c r="F106" s="33"/>
+      <c r="G106" s="33"/>
+      <c r="H106" s="33"/>
+      <c r="I106" s="33"/>
+      <c r="J106" s="33"/>
+      <c r="K106" s="33"/>
+    </row>
+    <row r="107" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="A7:K7"/>
+    <mergeCell ref="A106:K106"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="E18:G18"/>
+    <mergeCell ref="A56:K56"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="A14:K14"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="E16:G16"/>
     <mergeCell ref="B9:D9"/>
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="B10:D10"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="B11:D11"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="A14:K14"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="E16:G16"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="E18:G18"/>
-    <mergeCell ref="A56:K56"/>
-    <mergeCell ref="A106:K106"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="A7:K7"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="J3:K3"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
-  <pageMargins left="0.2362204724409449" right="0.2362204724409449" top="0.07874015748031496" bottom="0.3937007874015748" header="0.31496062992125984" footer="0.1968503937007874"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="90" fitToWidth="1" fitToHeight="0" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
+  <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="7.874015748031496E-2" bottom="1.1811023622047245" header="0.31496062992125984" footer="0.19685039370078741"/>
+  <pageSetup paperSize="9" scale="90" fitToHeight="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
   <headerFooter>
     <oddFooter>&amp;CС правом на технические изменения без предварительного уведомления.</oddFooter>
   </headerFooter>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>